<commit_message>
Bunch of headshots for Office Universe table
</commit_message>
<xml_diff>
--- a/halloween/office_costumes.xlsx
+++ b/halloween/office_costumes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\809projects\theoffice\halloween\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D037439-08F7-41FC-BD5F-1AC59E22E011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555F2411-36C7-4C73-8696-EE7F83882AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="153">
   <si>
     <t>character</t>
   </si>
@@ -377,9 +377,6 @@
   </si>
   <si>
     <t>Performer</t>
-  </si>
-  <si>
-    <t>Athlete</t>
   </si>
   <si>
     <t>Fictional character</t>
@@ -1324,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1346,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1420,7 +1417,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1437,7 +1434,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -1457,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -1477,7 +1474,7 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -1494,7 +1491,7 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -1511,7 +1508,7 @@
         <v>112</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -1528,7 +1525,7 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -1545,7 +1542,7 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -1562,7 +1559,7 @@
         <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -1582,7 +1579,7 @@
         <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -1596,10 +1593,10 @@
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -1633,7 +1630,7 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -1650,7 +1647,7 @@
         <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -1667,7 +1664,7 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -1678,13 +1675,13 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
         <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -1721,7 +1718,7 @@
         <v>108</v>
       </c>
       <c r="F22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -1741,7 +1738,7 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -1761,7 +1758,7 @@
         <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -1781,7 +1778,7 @@
         <v>34</v>
       </c>
       <c r="F25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -1801,7 +1798,7 @@
         <v>36</v>
       </c>
       <c r="F26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -1821,7 +1818,7 @@
         <v>39</v>
       </c>
       <c r="F27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -1838,7 +1835,7 @@
         <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -1855,7 +1852,7 @@
         <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -1875,7 +1872,7 @@
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -1895,7 +1892,7 @@
         <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -1912,7 +1909,7 @@
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -1926,10 +1923,10 @@
         <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -1943,10 +1940,10 @@
         <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -1963,7 +1960,7 @@
         <v>46</v>
       </c>
       <c r="F35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
@@ -1983,7 +1980,7 @@
         <v>48</v>
       </c>
       <c r="F36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -2000,7 +1997,7 @@
         <v>98</v>
       </c>
       <c r="F37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -2037,7 +2034,7 @@
         <v>51</v>
       </c>
       <c r="F39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -2057,7 +2054,7 @@
         <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
@@ -2074,7 +2071,7 @@
         <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -2094,7 +2091,7 @@
         <v>57</v>
       </c>
       <c r="F42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
@@ -2114,7 +2111,7 @@
         <v>59</v>
       </c>
       <c r="F43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -2128,10 +2125,10 @@
         <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
@@ -2148,7 +2145,7 @@
         <v>28</v>
       </c>
       <c r="F45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -2168,7 +2165,7 @@
         <v>61</v>
       </c>
       <c r="F46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -2182,7 +2179,7 @@
         <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F47" t="s">
         <v>118</v>
@@ -2205,7 +2202,7 @@
         <v>63</v>
       </c>
       <c r="F48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
@@ -2222,7 +2219,7 @@
         <v>65</v>
       </c>
       <c r="F49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
@@ -2236,13 +2233,13 @@
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
@@ -2259,7 +2256,7 @@
         <v>64</v>
       </c>
       <c r="F51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -2276,7 +2273,7 @@
         <v>66</v>
       </c>
       <c r="F52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
@@ -2296,7 +2293,7 @@
         <v>67</v>
       </c>
       <c r="F53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
@@ -2316,7 +2313,7 @@
         <v>67</v>
       </c>
       <c r="F54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
@@ -2353,7 +2350,7 @@
         <v>71</v>
       </c>
       <c r="F56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
@@ -2367,10 +2364,10 @@
         <v>31</v>
       </c>
       <c r="D57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
@@ -2401,10 +2398,10 @@
         <v>27</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
@@ -2424,7 +2421,7 @@
         <v>71</v>
       </c>
       <c r="F60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
@@ -2472,10 +2469,10 @@
         <v>55</v>
       </c>
       <c r="D63" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
@@ -2489,10 +2486,10 @@
         <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
@@ -2509,7 +2506,7 @@
         <v>116</v>
       </c>
       <c r="F65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
@@ -2523,10 +2520,10 @@
         <v>25</v>
       </c>
       <c r="D66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
@@ -2540,10 +2537,10 @@
         <v>29</v>
       </c>
       <c r="D67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
@@ -2557,10 +2554,10 @@
         <v>29</v>
       </c>
       <c r="D68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
@@ -2577,7 +2574,7 @@
         <v>28</v>
       </c>
       <c r="F69" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
@@ -2622,13 +2619,13 @@
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
@@ -2648,7 +2645,7 @@
         <v>78</v>
       </c>
       <c r="F73" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
@@ -2668,7 +2665,7 @@
         <v>67</v>
       </c>
       <c r="F74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
@@ -2685,7 +2682,7 @@
         <v>81</v>
       </c>
       <c r="F75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
@@ -2702,7 +2699,7 @@
         <v>82</v>
       </c>
       <c r="F76" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
@@ -2719,7 +2716,7 @@
         <v>83</v>
       </c>
       <c r="F77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
@@ -2736,7 +2733,7 @@
         <v>19</v>
       </c>
       <c r="F78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
@@ -2753,7 +2750,7 @@
         <v>84</v>
       </c>
       <c r="F79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
@@ -2770,7 +2767,7 @@
         <v>85</v>
       </c>
       <c r="F80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
@@ -2787,7 +2784,7 @@
         <v>86</v>
       </c>
       <c r="F81" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
@@ -2855,7 +2852,7 @@
         <v>90</v>
       </c>
       <c r="F85" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
@@ -2875,7 +2872,7 @@
         <v>92</v>
       </c>
       <c r="F86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
@@ -2895,7 +2892,7 @@
         <v>94</v>
       </c>
       <c r="F87" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
@@ -2912,7 +2909,7 @@
         <v>95</v>
       </c>
       <c r="F88" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
@@ -2929,7 +2926,7 @@
         <v>95</v>
       </c>
       <c r="F89" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
@@ -2946,7 +2943,7 @@
         <v>95</v>
       </c>
       <c r="F90" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
@@ -2960,13 +2957,13 @@
         <v>8</v>
       </c>
       <c r="D91" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E91" t="s">
         <v>96</v>
       </c>
       <c r="F91" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
@@ -3003,7 +3000,7 @@
         <v>99</v>
       </c>
       <c r="F93" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
@@ -3017,10 +3014,10 @@
         <v>8</v>
       </c>
       <c r="D94" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F94" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
@@ -3034,10 +3031,10 @@
         <v>8</v>
       </c>
       <c r="D95" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F95" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
@@ -3054,7 +3051,7 @@
         <v>100</v>
       </c>
       <c r="F96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
@@ -3068,10 +3065,10 @@
         <v>29</v>
       </c>
       <c r="D97" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F97" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
@@ -3085,10 +3082,10 @@
         <v>29</v>
       </c>
       <c r="D98" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
@@ -3105,7 +3102,7 @@
         <v>101</v>
       </c>
       <c r="F99" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
@@ -3119,10 +3116,10 @@
         <v>15</v>
       </c>
       <c r="D100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F100" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
@@ -3173,10 +3170,10 @@
         <v>105</v>
       </c>
       <c r="E103" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F103" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.45">
@@ -3193,7 +3190,7 @@
         <v>42</v>
       </c>
       <c r="F104" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.45">
@@ -3207,10 +3204,10 @@
         <v>31</v>
       </c>
       <c r="D105" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F105" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.45">
@@ -3227,7 +3224,7 @@
         <v>107</v>
       </c>
       <c r="F106" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
@@ -3241,10 +3238,10 @@
         <v>27</v>
       </c>
       <c r="D107" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
@@ -3258,10 +3255,10 @@
         <v>64</v>
       </c>
       <c r="D108" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F108" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Readying the blog post
</commit_message>
<xml_diff>
--- a/halloween/office_costumes.xlsx
+++ b/halloween/office_costumes.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\809projects\theoffice\halloween\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555F2411-36C7-4C73-8696-EE7F83882AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7143A2-3800-4718-8EDC-DE19643BCCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8" yWindow="8" windowWidth="20505" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="office_costumes_raw" sheetId="1" r:id="rId1"/>
+    <sheet name="within_universe" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="157">
   <si>
     <t>character</t>
   </si>
@@ -479,6 +480,18 @@
   </si>
   <si>
     <t>Zombie</t>
+  </si>
+  <si>
+    <t>dressed_as</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>episode</t>
+  </si>
+  <si>
+    <t>Jo</t>
   </si>
 </sst>
 </file>
@@ -1321,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3014,10 +3027,10 @@
         <v>8</v>
       </c>
       <c r="D94" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F94" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
@@ -3031,10 +3044,10 @@
         <v>8</v>
       </c>
       <c r="D95" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F95" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
@@ -3259,6 +3272,231 @@
       </c>
       <c r="F108" t="s">
         <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007048B6-1CD0-4ADC-9FDC-3A1B4139E3B2}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More prep for blog post
</commit_message>
<xml_diff>
--- a/halloween/office_costumes.xlsx
+++ b/halloween/office_costumes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\809projects\theoffice\halloween\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7143A2-3800-4718-8EDC-DE19643BCCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C2E613-8F04-4536-ACD8-093A7BFCF837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8" yWindow="8" windowWidth="20505" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="158">
   <si>
     <t>character</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>Jo</t>
+  </si>
+  <si>
+    <t>a Black Widow</t>
   </si>
 </sst>
 </file>
@@ -1334,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2007,7 +2010,7 @@
         <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="F37" t="s">
         <v>127</v>

</xml_diff>